<commit_message>
added more to compass files backend
</commit_message>
<xml_diff>
--- a/main/src/main/resources/org/example/Aggrigrated college sheet only 2024.xlsx
+++ b/main/src/main/resources/org/example/Aggrigrated college sheet only 2024.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="178">
   <si>
     <t>Name</t>
   </si>
@@ -31,9 +31,6 @@
     <t>Virtual resources</t>
   </si>
   <si>
-    <t>The College Tour video</t>
-  </si>
-  <si>
     <t>Ball State</t>
   </si>
   <si>
@@ -76,9 +73,6 @@
     <t>Butler</t>
   </si>
   <si>
-    <t>About Butler</t>
-  </si>
-  <si>
     <t>Cal Poly Humboldt</t>
   </si>
   <si>
@@ -91,9 +85,6 @@
     <t>Cal Poly SLO</t>
   </si>
   <si>
-    <t>Videos</t>
-  </si>
-  <si>
     <t>Cal state Channel Islands</t>
   </si>
   <si>
@@ -112,13 +103,13 @@
     <t>Coastal Carolina</t>
   </si>
   <si>
+    <t>Colorado State</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colorado State </t>
+  </si>
+  <si>
     <t>Virtual Tour</t>
-  </si>
-  <si>
-    <t>Colorado State</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Colorado State </t>
   </si>
   <si>
     <t>Colorado State University</t>
@@ -161,6 +152,9 @@
     <t>Florida State</t>
   </si>
   <si>
+    <t>Videos</t>
+  </si>
+  <si>
     <t>Fordham</t>
   </si>
   <si>
@@ -191,48 +185,48 @@
     <t>Hawaii Manoa</t>
   </si>
   <si>
+    <t>Indiana Bloomington</t>
+  </si>
+  <si>
+    <t>Kentucky</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KU- </t>
+  </si>
+  <si>
+    <t>Lewis and Clark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Louisville </t>
+  </si>
+  <si>
+    <t>Loyola Chicago</t>
+  </si>
+  <si>
+    <t>LSU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marquette </t>
+  </si>
+  <si>
+    <t>Miami of Ohio</t>
+  </si>
+  <si>
+    <t>Michigan State</t>
+  </si>
+  <si>
+    <t>Minnesota Stare Univerity- Mankato</t>
+  </si>
+  <si>
+    <t>Minnesota State Moorehead*</t>
+  </si>
+  <si>
+    <t>Montana State</t>
+  </si>
+  <si>
     <t>Watch Here</t>
   </si>
   <si>
-    <t>Indiana Bloomington</t>
-  </si>
-  <si>
-    <t>Kentucky</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KU- </t>
-  </si>
-  <si>
-    <t>Lewis and Clark</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Louisville </t>
-  </si>
-  <si>
-    <t>Loyola Chicago</t>
-  </si>
-  <si>
-    <t>LSU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marquette </t>
-  </si>
-  <si>
-    <t>Miami of Ohio</t>
-  </si>
-  <si>
-    <t>Michigan State</t>
-  </si>
-  <si>
-    <t>Minnesota Stare Univerity- Mankato</t>
-  </si>
-  <si>
-    <t>Minnesota State Moorehead*</t>
-  </si>
-  <si>
-    <t>Montana State</t>
-  </si>
-  <si>
     <t xml:space="preserve">Montana State </t>
   </si>
   <si>
@@ -299,169 +293,169 @@
     <t>Santa Clara</t>
   </si>
   <si>
+    <t>Santa Clara?</t>
+  </si>
+  <si>
+    <t>SDSU</t>
+  </si>
+  <si>
+    <t>Seattle University</t>
+  </si>
+  <si>
+    <t>SMU</t>
+  </si>
+  <si>
+    <t>Video and tour</t>
+  </si>
+  <si>
+    <t>St. Cloud State*</t>
+  </si>
+  <si>
+    <t>St. Louis University- 3+3 program</t>
+  </si>
+  <si>
+    <t>St. Mary's College of California</t>
+  </si>
+  <si>
+    <t>St. Norbert</t>
+  </si>
+  <si>
+    <t>Stanford</t>
+  </si>
+  <si>
+    <t>Stanford University</t>
+  </si>
+  <si>
+    <t>Syracuse University</t>
+  </si>
+  <si>
+    <t>TCU</t>
+  </si>
+  <si>
+    <t>Tennessee</t>
+  </si>
+  <si>
+    <t>Texas Christian</t>
+  </si>
+  <si>
+    <t>Texas Tech</t>
+  </si>
+  <si>
+    <t>Tufts</t>
+  </si>
+  <si>
+    <t>U of Minnesota - Twin Cities</t>
+  </si>
+  <si>
+    <t>U of Minnesota in Duluth</t>
+  </si>
+  <si>
+    <t>U of Minnesota- Morris</t>
+  </si>
+  <si>
+    <t>U of Wisconsin Green Bay</t>
+  </si>
+  <si>
+    <t>U of Wisconsin Lacrosse</t>
+  </si>
+  <si>
+    <t>U of Wisconsin Milwaukee</t>
+  </si>
+  <si>
+    <t>U of Wisconsin Oshkosh</t>
+  </si>
+  <si>
+    <t>UC Berkeley</t>
+  </si>
+  <si>
+    <t>UC Davis</t>
+  </si>
+  <si>
+    <t>UC Irvine</t>
+  </si>
+  <si>
+    <t>UC Santa Barbara</t>
+  </si>
+  <si>
+    <t>UC Santa Cruz</t>
+  </si>
+  <si>
+    <t>UCLA</t>
+  </si>
+  <si>
+    <t>UCSB</t>
+  </si>
+  <si>
+    <t>UCSD</t>
+  </si>
+  <si>
+    <t>UNC Wilmington</t>
+  </si>
+  <si>
+    <t>University Nevada Reno- WUE</t>
+  </si>
+  <si>
+    <t>University of Alabama</t>
+  </si>
+  <si>
+    <t>University of Alaska, Southeast</t>
+  </si>
+  <si>
+    <t>University of Arizona</t>
+  </si>
+  <si>
+    <t>University Of Cincinnati- 3+3 program</t>
+  </si>
+  <si>
+    <t>University of Cinicinnati</t>
+  </si>
+  <si>
+    <t>University of Colorado, Colorado Springs</t>
+  </si>
+  <si>
+    <t>University of Delaware</t>
+  </si>
+  <si>
+    <t>University of Florida</t>
+  </si>
+  <si>
+    <t>Photo Gallery</t>
+  </si>
+  <si>
+    <t>University of Hawaii</t>
+  </si>
+  <si>
+    <t>University of Hawaii Manoa</t>
+  </si>
+  <si>
+    <t>University of Hawaii Manoa- WUE</t>
+  </si>
+  <si>
+    <t>University of Iowa</t>
+  </si>
+  <si>
+    <t>HERE</t>
+  </si>
+  <si>
+    <t>University of Memphis- 3+3 program</t>
+  </si>
+  <si>
+    <t>University of Miami</t>
+  </si>
+  <si>
+    <t>University of Michigan</t>
+  </si>
+  <si>
+    <t>University of Nevada Reno</t>
+  </si>
+  <si>
+    <t>University of New Hampshire</t>
+  </si>
+  <si>
+    <t>University of Portland</t>
+  </si>
+  <si>
     <t>Video</t>
-  </si>
-  <si>
-    <t>Santa Clara?</t>
-  </si>
-  <si>
-    <t>SDSU</t>
-  </si>
-  <si>
-    <t>Seattle University</t>
-  </si>
-  <si>
-    <t>SMU</t>
-  </si>
-  <si>
-    <t>Video and tour</t>
-  </si>
-  <si>
-    <t>St. Cloud State*</t>
-  </si>
-  <si>
-    <t>St. Louis University- 3+3 program</t>
-  </si>
-  <si>
-    <t>St. Mary's College of California</t>
-  </si>
-  <si>
-    <t>St. Norbert</t>
-  </si>
-  <si>
-    <t>Stanford</t>
-  </si>
-  <si>
-    <t>Stanford University</t>
-  </si>
-  <si>
-    <t>Syracuse University</t>
-  </si>
-  <si>
-    <t>TCU</t>
-  </si>
-  <si>
-    <t>Tennessee</t>
-  </si>
-  <si>
-    <t>Texas Christian</t>
-  </si>
-  <si>
-    <t>Texas Tech</t>
-  </si>
-  <si>
-    <t>Tufts</t>
-  </si>
-  <si>
-    <t>U of Minnesota - Twin Cities</t>
-  </si>
-  <si>
-    <t>U of Minnesota in Duluth</t>
-  </si>
-  <si>
-    <t>U of Minnesota- Morris</t>
-  </si>
-  <si>
-    <t>U of Wisconsin Green Bay</t>
-  </si>
-  <si>
-    <t>U of Wisconsin Lacrosse</t>
-  </si>
-  <si>
-    <t>U of Wisconsin Milwaukee</t>
-  </si>
-  <si>
-    <t>U of Wisconsin Oshkosh</t>
-  </si>
-  <si>
-    <t>UC Berkeley</t>
-  </si>
-  <si>
-    <t>UC Davis</t>
-  </si>
-  <si>
-    <t>UC Irvine</t>
-  </si>
-  <si>
-    <t>UC Santa Barbara</t>
-  </si>
-  <si>
-    <t>UC Santa Cruz</t>
-  </si>
-  <si>
-    <t>UCLA</t>
-  </si>
-  <si>
-    <t>UCSB</t>
-  </si>
-  <si>
-    <t>UCSD</t>
-  </si>
-  <si>
-    <t>UNC Wilmington</t>
-  </si>
-  <si>
-    <t>University Nevada Reno- WUE</t>
-  </si>
-  <si>
-    <t>University of Alabama</t>
-  </si>
-  <si>
-    <t>University of Alaska, Southeast</t>
-  </si>
-  <si>
-    <t>University of Arizona</t>
-  </si>
-  <si>
-    <t>University Of Cincinnati- 3+3 program</t>
-  </si>
-  <si>
-    <t>University of Cinicinnati</t>
-  </si>
-  <si>
-    <t>University of Colorado, Colorado Springs</t>
-  </si>
-  <si>
-    <t>University of Delaware</t>
-  </si>
-  <si>
-    <t>University of Florida</t>
-  </si>
-  <si>
-    <t>Photo Gallery</t>
-  </si>
-  <si>
-    <t>University of Hawaii</t>
-  </si>
-  <si>
-    <t>University of Hawaii Manoa</t>
-  </si>
-  <si>
-    <t>University of Hawaii Manoa- WUE</t>
-  </si>
-  <si>
-    <t>University of Iowa</t>
-  </si>
-  <si>
-    <t>HERE</t>
-  </si>
-  <si>
-    <t>University of Memphis- 3+3 program</t>
-  </si>
-  <si>
-    <t>University of Miami</t>
-  </si>
-  <si>
-    <t>University of Michigan</t>
-  </si>
-  <si>
-    <t>University of Nevada Reno</t>
-  </si>
-  <si>
-    <t>University of New Hampshire</t>
-  </si>
-  <si>
-    <t>University of Portland</t>
   </si>
   <si>
     <t>University of Redlands</t>
@@ -858,7 +852,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>3</v>
@@ -866,15 +860,15 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>3</v>
@@ -882,55 +876,55 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="s">
-        <v>10</v>
+      <c r="A8" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="4" t="s">
-        <v>13</v>
+      <c r="A10" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>3</v>
@@ -938,55 +932,55 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>3</v>
@@ -994,15 +988,15 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>3</v>
@@ -1010,7 +1004,7 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>3</v>
@@ -1018,63 +1012,63 @@
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>3</v>
@@ -1082,95 +1076,95 @@
     </row>
     <row r="32">
       <c r="A32" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>33</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>33</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>37</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>3</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>3</v>
@@ -1178,23 +1172,23 @@
     </row>
     <row r="44">
       <c r="A44" s="2" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>3</v>
@@ -1202,15 +1196,15 @@
     </row>
     <row r="47">
       <c r="A47" s="2" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>3</v>
@@ -1218,15 +1212,15 @@
     </row>
     <row r="49">
       <c r="A49" s="2" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>3</v>
@@ -1234,15 +1228,15 @@
     </row>
     <row r="51">
       <c r="A51" s="2" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>3</v>
@@ -1250,71 +1244,71 @@
     </row>
     <row r="53">
       <c r="A53" s="2" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="2" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>59</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="2" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="2" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>3</v>
+        <v>70</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="2" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="2" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="2" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>3</v>
@@ -1322,47 +1316,47 @@
     </row>
     <row r="62">
       <c r="A62" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="2" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="2" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="2" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="2" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="2" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>3</v>
@@ -1370,7 +1364,7 @@
     </row>
     <row r="68">
       <c r="A68" s="2" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>3</v>
@@ -1378,95 +1372,95 @@
     </row>
     <row r="69">
       <c r="A69" s="2" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="2" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="2" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="2" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="2" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="2" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>3</v>
+        <v>46</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="2" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="2" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="2" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="2" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="2" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="2" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>3</v>
@@ -1474,71 +1468,71 @@
     </row>
     <row r="81">
       <c r="A81" s="2" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="2" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="2" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="2" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>39</v>
+        <v>97</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="2" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="2" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="2" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="2" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="2" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>3</v>
@@ -1546,39 +1540,39 @@
     </row>
     <row r="90">
       <c r="A90" s="2" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="2" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="2" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="2" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="2" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>3</v>
@@ -1586,95 +1580,95 @@
     </row>
     <row r="95">
       <c r="A95" s="2" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>95</v>
+        <v>3</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="2" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="2" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="2" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="2" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="2" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>100</v>
+        <v>11</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="2" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="2" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="2" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="2" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="2" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="2" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>3</v>
@@ -1682,135 +1676,135 @@
     </row>
     <row r="107">
       <c r="A107" s="2" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="2" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="2" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="2" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="2" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>33</v>
+        <v>3</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="2" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="2" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="2" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="2" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="2" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="2" t="s">
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="2" t="s">
-        <v>116</v>
+        <v>131</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="2" t="s">
-        <v>117</v>
+        <v>132</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="2" t="s">
-        <v>118</v>
+        <v>133</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="2" t="s">
-        <v>119</v>
+        <v>134</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>3</v>
+        <v>135</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="2" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="2" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="B123" s="3" t="s">
         <v>3</v>
@@ -1818,31 +1812,31 @@
     </row>
     <row r="124">
       <c r="A124" s="2" t="s">
-        <v>121</v>
+        <v>138</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="2" t="s">
-        <v>122</v>
+        <v>139</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>3</v>
+        <v>140</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="2" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="2" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="B127" s="3" t="s">
         <v>3</v>
@@ -1850,79 +1844,79 @@
     </row>
     <row r="128">
       <c r="A128" s="2" t="s">
-        <v>124</v>
+        <v>143</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="2" t="s">
-        <v>125</v>
+        <v>144</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="2" t="s">
-        <v>125</v>
+        <v>145</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="2" t="s">
-        <v>126</v>
+        <v>146</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>9</v>
+        <v>147</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="2" t="s">
-        <v>126</v>
+        <v>148</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="2" t="s">
-        <v>127</v>
+        <v>149</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="2" t="s">
-        <v>128</v>
+        <v>150</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="2" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>3</v>
+        <v>152</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="2" t="s">
-        <v>129</v>
+        <v>153</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="2" t="s">
-        <v>130</v>
+        <v>154</v>
       </c>
       <c r="B137" s="3" t="s">
         <v>3</v>
@@ -1930,15 +1924,15 @@
     </row>
     <row r="138">
       <c r="A138" s="2" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>33</v>
+        <v>3</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="2" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
       <c r="B139" s="3" t="s">
         <v>3</v>
@@ -1946,15 +1940,15 @@
     </row>
     <row r="140">
       <c r="A140" s="2" t="s">
-        <v>132</v>
+        <v>157</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="2" t="s">
-        <v>132</v>
+        <v>158</v>
       </c>
       <c r="B141" s="3" t="s">
         <v>3</v>
@@ -1962,15 +1956,15 @@
     </row>
     <row r="142">
       <c r="A142" s="2" t="s">
-        <v>133</v>
+        <v>159</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="2" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="B143" s="3" t="s">
         <v>3</v>
@@ -1978,7 +1972,7 @@
     </row>
     <row r="144">
       <c r="A144" s="2" t="s">
-        <v>135</v>
+        <v>161</v>
       </c>
       <c r="B144" s="3" t="s">
         <v>3</v>
@@ -1986,63 +1980,63 @@
     </row>
     <row r="145">
       <c r="A145" s="2" t="s">
-        <v>136</v>
+        <v>162</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>3</v>
+        <v>46</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="2" t="s">
-        <v>137</v>
+        <v>163</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>138</v>
+        <v>3</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="2" t="s">
-        <v>139</v>
+        <v>164</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="2" t="s">
-        <v>140</v>
+        <v>165</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="2" t="s">
-        <v>141</v>
+        <v>166</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="2" t="s">
-        <v>142</v>
+        <v>167</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>143</v>
+        <v>70</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="2" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="2" t="s">
-        <v>145</v>
+        <v>169</v>
       </c>
       <c r="B152" s="3" t="s">
         <v>3</v>
@@ -2050,305 +2044,65 @@
     </row>
     <row r="153">
       <c r="A153" s="2" t="s">
-        <v>146</v>
+        <v>170</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="2" t="s">
-        <v>147</v>
+        <v>171</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>33</v>
+        <v>3</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="2" t="s">
-        <v>148</v>
+        <v>172</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="2" t="s">
-        <v>149</v>
+        <v>173</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>95</v>
+        <v>3</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="2" t="s">
-        <v>149</v>
+        <v>174</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="2" t="s">
-        <v>150</v>
+        <v>175</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="2" t="s">
-        <v>151</v>
+        <v>176</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="2" t="s">
-        <v>152</v>
+        <v>177</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="161">
-      <c r="A161" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="B161" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="162">
-      <c r="A162" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="B162" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="163">
-      <c r="A163" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="B163" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="164">
-      <c r="A164" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B164" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="165">
-      <c r="A165" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="B165" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="166">
-      <c r="A166" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="B166" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="167">
-      <c r="A167" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="B167" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="168">
-      <c r="A168" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="B168" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="169">
-      <c r="A169" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="B169" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="170">
-      <c r="A170" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="B170" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="171">
-      <c r="A171" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="B171" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="172">
-      <c r="A172" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="B172" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="173">
-      <c r="A173" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="B173" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="174">
-      <c r="A174" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="B174" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="175">
-      <c r="A175" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="B175" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="176">
-      <c r="A176" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="B176" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="177">
-      <c r="A177" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="B177" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="178">
-      <c r="A178" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="B178" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="179">
-      <c r="A179" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="B179" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="180">
-      <c r="A180" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="B180" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="181">
-      <c r="A181" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="B181" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="182">
-      <c r="A182" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="B182" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="B183" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="184">
-      <c r="A184" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B184" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="185">
-      <c r="A185" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="B185" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="186">
-      <c r="A186" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="B186" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="187">
-      <c r="A187" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="B187" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="188">
-      <c r="A188" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="B188" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="189">
-      <c r="A189" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B189" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="190">
-      <c r="A190" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="B190" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2413,21 +2167,21 @@
     <hyperlink r:id="rId54" ref="B55"/>
     <hyperlink r:id="rId55" ref="B56"/>
     <hyperlink r:id="rId56" ref="B57"/>
-    <hyperlink r:id="rId57" ref="B58"/>
-    <hyperlink r:id="rId58" ref="B59"/>
+    <hyperlink r:id="rId57" location="virtualtour" ref="B58"/>
+    <hyperlink r:id="rId58" location="tours" ref="B59"/>
     <hyperlink r:id="rId59" ref="B60"/>
     <hyperlink r:id="rId60" ref="B61"/>
-    <hyperlink r:id="rId61" location="virtualtour" ref="B62"/>
+    <hyperlink r:id="rId61" ref="B62"/>
     <hyperlink r:id="rId62" ref="B63"/>
     <hyperlink r:id="rId63" ref="B64"/>
-    <hyperlink r:id="rId64" location="virtualtour" ref="B65"/>
+    <hyperlink r:id="rId64" ref="B65"/>
     <hyperlink r:id="rId65" ref="B66"/>
     <hyperlink r:id="rId66" ref="B67"/>
     <hyperlink r:id="rId67" ref="B68"/>
     <hyperlink r:id="rId68" ref="B69"/>
     <hyperlink r:id="rId69" ref="B70"/>
-    <hyperlink r:id="rId70" location="virtualtour" ref="B71"/>
-    <hyperlink r:id="rId71" location="tours" ref="B72"/>
+    <hyperlink r:id="rId70" ref="B71"/>
+    <hyperlink r:id="rId71" ref="B72"/>
     <hyperlink r:id="rId72" ref="B73"/>
     <hyperlink r:id="rId73" ref="B74"/>
     <hyperlink r:id="rId74" ref="B75"/>
@@ -2453,7 +2207,7 @@
     <hyperlink r:id="rId94" ref="B95"/>
     <hyperlink r:id="rId95" ref="B96"/>
     <hyperlink r:id="rId96" ref="B97"/>
-    <hyperlink r:id="rId97" ref="B98"/>
+    <hyperlink r:id="rId97" location="!ct/?s/" ref="B98"/>
     <hyperlink r:id="rId98" ref="B99"/>
     <hyperlink r:id="rId99" ref="B100"/>
     <hyperlink r:id="rId100" ref="B101"/>
@@ -2465,13 +2219,13 @@
     <hyperlink r:id="rId106" ref="B107"/>
     <hyperlink r:id="rId107" ref="B108"/>
     <hyperlink r:id="rId108" ref="B109"/>
-    <hyperlink r:id="rId109" ref="B110"/>
+    <hyperlink r:id="rId109" location=":~:text=Guided%20Virtual%20Tours,available%20options%20and%20register%20below." ref="B110"/>
     <hyperlink r:id="rId110" ref="B111"/>
     <hyperlink r:id="rId111" ref="B112"/>
     <hyperlink r:id="rId112" ref="B113"/>
     <hyperlink r:id="rId113" ref="B114"/>
     <hyperlink r:id="rId114" ref="B115"/>
-    <hyperlink r:id="rId115" location="!ct/?s/" ref="B116"/>
+    <hyperlink r:id="rId115" ref="B116"/>
     <hyperlink r:id="rId116" ref="B117"/>
     <hyperlink r:id="rId117" ref="B118"/>
     <hyperlink r:id="rId118" ref="B119"/>
@@ -2486,7 +2240,7 @@
     <hyperlink r:id="rId127" ref="B128"/>
     <hyperlink r:id="rId128" ref="B129"/>
     <hyperlink r:id="rId129" ref="B130"/>
-    <hyperlink r:id="rId130" location=":~:text=Guided%20Virtual%20Tours,available%20options%20and%20register%20below." ref="B131"/>
+    <hyperlink r:id="rId130" ref="B131"/>
     <hyperlink r:id="rId131" ref="B132"/>
     <hyperlink r:id="rId132" ref="B133"/>
     <hyperlink r:id="rId133" ref="B134"/>
@@ -2495,7 +2249,7 @@
     <hyperlink r:id="rId136" ref="B137"/>
     <hyperlink r:id="rId137" ref="B138"/>
     <hyperlink r:id="rId138" ref="B139"/>
-    <hyperlink r:id="rId139" ref="B140"/>
+    <hyperlink r:id="rId139" location="virtualtour" ref="B140"/>
     <hyperlink r:id="rId140" ref="B141"/>
     <hyperlink r:id="rId141" ref="B142"/>
     <hyperlink r:id="rId142" ref="B143"/>
@@ -2516,37 +2270,7 @@
     <hyperlink r:id="rId157" ref="B158"/>
     <hyperlink r:id="rId158" ref="B159"/>
     <hyperlink r:id="rId159" ref="B160"/>
-    <hyperlink r:id="rId160" ref="B161"/>
-    <hyperlink r:id="rId161" ref="B162"/>
-    <hyperlink r:id="rId162" ref="B163"/>
-    <hyperlink r:id="rId163" ref="B164"/>
-    <hyperlink r:id="rId164" ref="B165"/>
-    <hyperlink r:id="rId165" ref="B166"/>
-    <hyperlink r:id="rId166" ref="B167"/>
-    <hyperlink r:id="rId167" location="virtualtour" ref="B168"/>
-    <hyperlink r:id="rId168" ref="B169"/>
-    <hyperlink r:id="rId169" ref="B170"/>
-    <hyperlink r:id="rId170" ref="B171"/>
-    <hyperlink r:id="rId171" ref="B172"/>
-    <hyperlink r:id="rId172" ref="B173"/>
-    <hyperlink r:id="rId173" ref="B174"/>
-    <hyperlink r:id="rId174" ref="B175"/>
-    <hyperlink r:id="rId175" ref="B176"/>
-    <hyperlink r:id="rId176" ref="B177"/>
-    <hyperlink r:id="rId177" ref="B178"/>
-    <hyperlink r:id="rId178" ref="B179"/>
-    <hyperlink r:id="rId179" ref="B180"/>
-    <hyperlink r:id="rId180" ref="B181"/>
-    <hyperlink r:id="rId181" ref="B182"/>
-    <hyperlink r:id="rId182" ref="B183"/>
-    <hyperlink r:id="rId183" ref="B184"/>
-    <hyperlink r:id="rId184" ref="B185"/>
-    <hyperlink r:id="rId185" ref="B186"/>
-    <hyperlink r:id="rId186" ref="B187"/>
-    <hyperlink r:id="rId187" ref="B188"/>
-    <hyperlink r:id="rId188" ref="B189"/>
-    <hyperlink r:id="rId189" ref="B190"/>
   </hyperlinks>
-  <drawing r:id="rId190"/>
+  <drawing r:id="rId160"/>
 </worksheet>
 </file>
</xml_diff>